<commit_message>
added arguments to functions in libplot. fixed test script.
</commit_message>
<xml_diff>
--- a/test_data/E-chem data (auto backup) - Copy2/LCO_Echem_data_summary.xlsx
+++ b/test_data/E-chem data (auto backup) - Copy2/LCO_Echem_data_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jzxiang\libedp\test_data\E-chem data (auto backup) - Copy2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC602345-6F08-4F51-A26A-E770D7EA0074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F804257-5CD7-4B18-AEBD-4559E2C55908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="79">
   <si>
     <t>Date</t>
   </si>
@@ -223,9 +223,6 @@
     <t>1-1-2818575870</t>
   </si>
   <si>
-    <t>3-3-2818575870</t>
-  </si>
-  <si>
     <t>5-5-2818575870</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
   </si>
   <si>
     <t>PNE-LCO-255i</t>
-  </si>
-  <si>
-    <t>1-3-2818575871</t>
   </si>
   <si>
     <t>2-4-2818575871</t>
@@ -856,29 +850,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="37">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1502,11 +1474,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK673"/>
+  <dimension ref="A1:AK671"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B317" sqref="B317"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -1677,18 +1649,18 @@
         <v>91.840999999999994</v>
       </c>
       <c r="N2" s="40">
-        <f t="shared" ref="N2:N19" si="0">K2/J2</f>
+        <f t="shared" ref="N2:N17" si="0">K2/J2</f>
         <v>157.1977949930706</v>
       </c>
       <c r="O2" s="40">
-        <f t="shared" ref="O2:O19" si="1">L2/J2</f>
+        <f t="shared" ref="O2:O17" si="1">L2/J2</f>
         <v>144.37179791510502</v>
       </c>
       <c r="P2" s="43">
         <v>5.5750999999999999</v>
       </c>
       <c r="Q2" s="32">
-        <f t="shared" ref="Q2:Q9" si="2">P2/J2</f>
+        <f t="shared" ref="Q2:Q8" si="2">P2/J2</f>
         <v>570.68009823915338</v>
       </c>
       <c r="R2" s="32"/>
@@ -1730,35 +1702,37 @@
       </c>
       <c r="F3" s="87"/>
       <c r="G3" s="35" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I3" s="38">
-        <v>1.9099999999999999E-2</v>
+        <v>1.9199999999999998E-2</v>
       </c>
       <c r="J3" s="23">
-        <v>9.7692209999999998E-3</v>
+        <v>9.8461439999999994E-3</v>
       </c>
       <c r="K3" s="10">
-        <v>0</v>
+        <v>1.5701000000000001</v>
       </c>
       <c r="L3" s="9">
-        <v>0</v>
+        <v>1.4184000000000001</v>
       </c>
       <c r="M3" s="40">
-        <v>0</v>
+        <v>90.337000000000003</v>
       </c>
       <c r="N3" s="40">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>159.46344071344072</v>
       </c>
       <c r="O3" s="40">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P3" s="43"/>
+        <v>144.05639405639408</v>
+      </c>
+      <c r="P3" s="43">
+        <v>5.6075999999999997</v>
+      </c>
       <c r="Q3" s="32">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>569.52244452244452</v>
       </c>
       <c r="R3" s="32"/>
       <c r="S3" s="9"/>
@@ -1792,7 +1766,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="93" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="E4" s="51" t="s">
         <v>15</v>
@@ -1802,34 +1776,34 @@
         <v>65</v>
       </c>
       <c r="I4" s="38">
-        <v>1.9199999999999998E-2</v>
+        <v>2.12E-2</v>
       </c>
       <c r="J4" s="23">
-        <v>9.8461439999999994E-3</v>
+        <v>1.1384604E-2</v>
       </c>
       <c r="K4" s="10">
-        <v>1.5701000000000001</v>
+        <v>1.8403</v>
       </c>
       <c r="L4" s="9">
-        <v>1.4184000000000001</v>
+        <v>1.6181000000000001</v>
       </c>
       <c r="M4" s="40">
-        <v>90.337000000000003</v>
+        <v>87.924000000000007</v>
       </c>
       <c r="N4" s="40">
         <f t="shared" si="0"/>
-        <v>159.46344071344072</v>
+        <v>161.6481346211076</v>
       </c>
       <c r="O4" s="40">
         <f t="shared" si="1"/>
-        <v>144.05639405639408</v>
+        <v>142.13054753595296</v>
       </c>
       <c r="P4" s="43">
-        <v>5.6075999999999997</v>
+        <v>6.3990999999999998</v>
       </c>
       <c r="Q4" s="32">
         <f t="shared" si="2"/>
-        <v>569.52244452244452</v>
+        <v>562.08367019177831</v>
       </c>
       <c r="R4" s="32"/>
       <c r="S4" s="9"/>
@@ -1873,34 +1847,34 @@
         <v>66</v>
       </c>
       <c r="I5" s="38">
-        <v>2.12E-2</v>
+        <v>2.1600000000000001E-2</v>
       </c>
       <c r="J5" s="23">
-        <v>1.1384604E-2</v>
+        <v>1.1692296000000001E-2</v>
       </c>
       <c r="K5" s="10">
-        <v>1.8403</v>
+        <v>1.7914000000000001</v>
       </c>
       <c r="L5" s="9">
-        <v>1.6181000000000001</v>
+        <v>1.6717</v>
       </c>
       <c r="M5" s="40">
-        <v>87.924000000000007</v>
+        <v>93.316999999999993</v>
       </c>
       <c r="N5" s="40">
         <f t="shared" si="0"/>
-        <v>161.6481346211076</v>
+        <v>153.21199531725847</v>
       </c>
       <c r="O5" s="40">
         <f t="shared" si="1"/>
-        <v>142.13054753595296</v>
+        <v>142.97448507974821</v>
       </c>
       <c r="P5" s="43">
-        <v>6.3990999999999998</v>
+        <v>6.5918999999999999</v>
       </c>
       <c r="Q5" s="32">
         <f t="shared" si="2"/>
-        <v>562.08367019177831</v>
+        <v>563.78148483411633</v>
       </c>
       <c r="R5" s="32"/>
       <c r="S5" s="9"/>
@@ -1944,34 +1918,34 @@
         <v>67</v>
       </c>
       <c r="I6" s="38">
-        <v>2.1600000000000001E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="J6" s="23">
-        <v>1.1692296000000001E-2</v>
+        <v>1.1230758E-2</v>
       </c>
       <c r="K6" s="10">
-        <v>1.7914000000000001</v>
+        <v>1.8775999999999999</v>
       </c>
       <c r="L6" s="9">
-        <v>1.6717</v>
+        <v>1.6584000000000001</v>
       </c>
       <c r="M6" s="40">
-        <v>93.316999999999993</v>
+        <v>88.328000000000003</v>
       </c>
       <c r="N6" s="40">
         <f t="shared" si="0"/>
-        <v>153.21199531725847</v>
+        <v>167.18372882756444</v>
       </c>
       <c r="O6" s="40">
         <f t="shared" si="1"/>
-        <v>142.97448507974821</v>
+        <v>147.66590109055863</v>
       </c>
       <c r="P6" s="43">
-        <v>6.5918999999999999</v>
+        <v>6.5590000000000002</v>
       </c>
       <c r="Q6" s="32">
         <f t="shared" si="2"/>
-        <v>563.78148483411633</v>
+        <v>584.02113196633741</v>
       </c>
       <c r="R6" s="32"/>
       <c r="S6" s="9"/>
@@ -2005,44 +1979,44 @@
         <v>14</v>
       </c>
       <c r="D7" s="93" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E7" s="51" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="F7" s="87"/>
       <c r="G7" s="35" t="s">
         <v>68</v>
       </c>
       <c r="I7" s="38">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1600000000000001E-2</v>
       </c>
       <c r="J7" s="23">
-        <v>1.1230758E-2</v>
+        <v>1.1692296000000001E-2</v>
       </c>
       <c r="K7" s="10">
-        <v>1.8775999999999999</v>
+        <v>1.744</v>
       </c>
       <c r="L7" s="9">
-        <v>1.6584000000000001</v>
+        <v>1.6095999999999999</v>
       </c>
       <c r="M7" s="40">
-        <v>88.328000000000003</v>
+        <v>92.293000000000006</v>
       </c>
       <c r="N7" s="40">
         <f t="shared" si="0"/>
-        <v>167.18372882756444</v>
+        <v>149.15804389488599</v>
       </c>
       <c r="O7" s="40">
         <f t="shared" si="1"/>
-        <v>147.66590109055863</v>
+        <v>137.66329555803239</v>
       </c>
       <c r="P7" s="43">
-        <v>6.5590000000000002</v>
+        <v>6.3472999999999997</v>
       </c>
       <c r="Q7" s="32">
         <f t="shared" si="2"/>
-        <v>584.02113196633741</v>
+        <v>542.8617270722533</v>
       </c>
       <c r="R7" s="32"/>
       <c r="S7" s="9"/>
@@ -2086,34 +2060,34 @@
         <v>69</v>
       </c>
       <c r="I8" s="38">
-        <v>2.1600000000000001E-2</v>
+        <v>2.0199999999999999E-2</v>
       </c>
       <c r="J8" s="23">
-        <v>1.1692296000000001E-2</v>
+        <v>1.0615373999999999E-2</v>
       </c>
       <c r="K8" s="10">
-        <v>1.744</v>
+        <v>1.6718</v>
       </c>
       <c r="L8" s="9">
-        <v>1.6095999999999999</v>
+        <v>1.4491000000000001</v>
       </c>
       <c r="M8" s="40">
-        <v>92.293000000000006</v>
+        <v>86.68</v>
       </c>
       <c r="N8" s="40">
         <f t="shared" si="0"/>
-        <v>149.15804389488599</v>
+        <v>157.48856328566475</v>
       </c>
       <c r="O8" s="40">
         <f t="shared" si="1"/>
-        <v>137.66329555803239</v>
+        <v>136.50955679941188</v>
       </c>
       <c r="P8" s="43">
-        <v>6.3472999999999997</v>
+        <v>5.7157999999999998</v>
       </c>
       <c r="Q8" s="32">
         <f t="shared" si="2"/>
-        <v>542.8617270722533</v>
+        <v>538.44546598169791</v>
       </c>
       <c r="R8" s="32"/>
       <c r="S8" s="9"/>
@@ -2154,37 +2128,37 @@
       </c>
       <c r="F9" s="87"/>
       <c r="G9" s="35" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="I9" s="38">
-        <v>2.0199999999999999E-2</v>
+        <v>2.0899999999999998E-2</v>
       </c>
       <c r="J9" s="23">
-        <v>1.0615373999999999E-2</v>
+        <v>1.1153834999999999E-2</v>
       </c>
       <c r="K9" s="10">
-        <v>1.6718</v>
+        <v>1.6040000000000001</v>
       </c>
       <c r="L9" s="9">
-        <v>1.4491000000000001</v>
+        <v>1.4862</v>
       </c>
       <c r="M9" s="40">
-        <v>86.68</v>
+        <v>92.956999999999994</v>
       </c>
       <c r="N9" s="40">
         <f t="shared" si="0"/>
-        <v>157.48856328566475</v>
+        <v>143.80704035876451</v>
       </c>
       <c r="O9" s="40">
         <f t="shared" si="1"/>
-        <v>136.50955679941188</v>
+        <v>133.24565048702979</v>
       </c>
       <c r="P9" s="43">
-        <v>5.7157999999999998</v>
+        <v>5.8484999999999996</v>
       </c>
       <c r="Q9" s="32">
-        <f t="shared" si="2"/>
-        <v>538.44546598169791</v>
+        <f t="shared" ref="Q9:Q17" si="3">P9/J9</f>
+        <v>524.34880021086917</v>
       </c>
       <c r="R9" s="32"/>
       <c r="S9" s="9"/>
@@ -2218,44 +2192,44 @@
         <v>14</v>
       </c>
       <c r="D10" s="93" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E10" s="51" t="s">
         <v>47</v>
       </c>
       <c r="F10" s="87"/>
       <c r="G10" s="35" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I10" s="38">
-        <v>2.0899999999999998E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="J10" s="23">
-        <v>1.1153834999999999E-2</v>
+        <v>9.6922980000000002E-3</v>
       </c>
       <c r="K10" s="10">
-        <v>1.6040000000000001</v>
+        <v>1.5879000000000001</v>
       </c>
       <c r="L10" s="9">
-        <v>1.4862</v>
+        <v>1.4092</v>
       </c>
       <c r="M10" s="40">
-        <v>92.956999999999994</v>
+        <v>88.751000000000005</v>
       </c>
       <c r="N10" s="40">
         <f t="shared" si="0"/>
-        <v>143.80704035876451</v>
+        <v>163.83111621206859</v>
       </c>
       <c r="O10" s="40">
         <f t="shared" si="1"/>
-        <v>133.24565048702979</v>
+        <v>145.39379618744698</v>
       </c>
       <c r="P10" s="43">
-        <v>5.8484999999999996</v>
+        <v>5.5667</v>
       </c>
       <c r="Q10" s="32">
-        <f t="shared" ref="Q10:Q19" si="3">P10/J10</f>
-        <v>524.34880021086917</v>
+        <f t="shared" si="3"/>
+        <v>574.34263783470135</v>
       </c>
       <c r="R10" s="32"/>
       <c r="S10" s="9"/>
@@ -2299,34 +2273,34 @@
         <v>71</v>
       </c>
       <c r="I11" s="38">
-        <v>1.9E-2</v>
+        <v>1.9400000000000001E-2</v>
       </c>
       <c r="J11" s="23">
-        <v>9.6922980000000002E-3</v>
+        <v>9.9999900000000003E-3</v>
       </c>
       <c r="K11" s="10">
-        <v>1.5879000000000001</v>
+        <v>1.5474000000000001</v>
       </c>
       <c r="L11" s="9">
-        <v>1.4092</v>
+        <v>1.4003000000000001</v>
       </c>
       <c r="M11" s="40">
-        <v>88.751000000000005</v>
+        <v>90.491</v>
       </c>
       <c r="N11" s="40">
         <f t="shared" si="0"/>
-        <v>163.83111621206859</v>
+        <v>154.74015474015474</v>
       </c>
       <c r="O11" s="40">
         <f t="shared" si="1"/>
-        <v>145.39379618744698</v>
+        <v>140.03014003014005</v>
       </c>
       <c r="P11" s="43">
-        <v>5.5667</v>
+        <v>5.5323000000000002</v>
       </c>
       <c r="Q11" s="32">
         <f t="shared" si="3"/>
-        <v>574.34263783470135</v>
+        <v>553.23055323055326</v>
       </c>
       <c r="R11" s="32"/>
       <c r="S11" s="9"/>
@@ -2349,148 +2323,147 @@
       <c r="AJ11" s="11"/>
       <c r="AK11" s="11"/>
     </row>
-    <row r="12" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="50">
+    <row r="12" spans="1:37" s="65" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="71">
         <v>44546</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="93" t="s">
+      <c r="D12" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="87"/>
-      <c r="G12" s="35" t="s">
+      <c r="F12" s="74"/>
+      <c r="G12" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="36"/>
+      <c r="I12" s="20">
+        <v>1.95E-2</v>
+      </c>
+      <c r="J12" s="24">
+        <v>1.0076913E-2</v>
+      </c>
+      <c r="K12" s="19">
+        <v>1.5612999999999999</v>
+      </c>
+      <c r="L12" s="18">
+        <v>1.4346000000000001</v>
+      </c>
+      <c r="M12" s="41">
+        <v>91.885999999999996</v>
+      </c>
+      <c r="N12" s="41">
+        <f t="shared" si="0"/>
+        <v>154.93832287725417</v>
+      </c>
+      <c r="O12" s="41">
+        <f t="shared" si="1"/>
+        <v>142.36502786121108</v>
+      </c>
+      <c r="P12" s="44">
+        <v>5.6696</v>
+      </c>
+      <c r="Q12" s="33">
+        <f t="shared" si="3"/>
+        <v>562.632623701326</v>
+      </c>
+      <c r="R12" s="33"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="18"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="20"/>
+      <c r="AD12" s="20"/>
+      <c r="AE12" s="20"/>
+      <c r="AF12" s="20"/>
+      <c r="AG12" s="20"/>
+      <c r="AH12" s="20"/>
+      <c r="AI12" s="20"/>
+      <c r="AJ12" s="20"/>
+      <c r="AK12" s="20"/>
+    </row>
+    <row r="13" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="50">
+        <v>44552</v>
+      </c>
+      <c r="B13" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="93" t="s">
         <v>72</v>
-      </c>
-      <c r="I12" s="38">
-        <v>1.9400000000000001E-2</v>
-      </c>
-      <c r="J12" s="23">
-        <v>9.9999900000000003E-3</v>
-      </c>
-      <c r="K12" s="10">
-        <v>1.5474000000000001</v>
-      </c>
-      <c r="L12" s="9">
-        <v>1.4003000000000001</v>
-      </c>
-      <c r="M12" s="40">
-        <v>90.491</v>
-      </c>
-      <c r="N12" s="40">
-        <f t="shared" si="0"/>
-        <v>154.74015474015474</v>
-      </c>
-      <c r="O12" s="40">
-        <f t="shared" si="1"/>
-        <v>140.03014003014005</v>
-      </c>
-      <c r="P12" s="43">
-        <v>5.5323000000000002</v>
-      </c>
-      <c r="Q12" s="32">
-        <f t="shared" si="3"/>
-        <v>553.23055323055326</v>
-      </c>
-      <c r="R12" s="32"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="38"/>
-      <c r="V12" s="38"/>
-      <c r="W12" s="38"/>
-      <c r="X12" s="38"/>
-      <c r="Y12" s="38"/>
-      <c r="Z12" s="38"/>
-      <c r="AA12" s="38"/>
-      <c r="AB12" s="38"/>
-      <c r="AC12" s="38"/>
-      <c r="AD12" s="11"/>
-      <c r="AE12" s="11"/>
-      <c r="AF12" s="11"/>
-      <c r="AG12" s="11"/>
-      <c r="AH12" s="11"/>
-      <c r="AI12" s="11"/>
-      <c r="AJ12" s="11"/>
-      <c r="AK12" s="11"/>
-    </row>
-    <row r="13" spans="1:37" s="65" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="71">
-        <v>44546</v>
-      </c>
-      <c r="B13" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="94" t="s">
-        <v>60</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="74"/>
-      <c r="G13" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="36"/>
-      <c r="I13" s="20">
-        <v>1.95E-2</v>
-      </c>
-      <c r="J13" s="24">
-        <v>1.0076913E-2</v>
-      </c>
-      <c r="K13" s="19">
-        <v>1.5612999999999999</v>
-      </c>
-      <c r="L13" s="18">
-        <v>1.4346000000000001</v>
-      </c>
-      <c r="M13" s="41">
-        <v>91.885999999999996</v>
-      </c>
-      <c r="N13" s="41">
+      <c r="G13" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" s="38">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="J13" s="23">
+        <v>1.728E-2</v>
+      </c>
+      <c r="K13" s="10">
+        <v>3.4662000000000002</v>
+      </c>
+      <c r="L13" s="9">
+        <v>3.0377000000000001</v>
+      </c>
+      <c r="M13" s="40">
+        <v>87.638000000000005</v>
+      </c>
+      <c r="N13" s="40">
         <f t="shared" si="0"/>
-        <v>154.93832287725417</v>
-      </c>
-      <c r="O13" s="41">
+        <v>200.59027777777777</v>
+      </c>
+      <c r="O13" s="40">
         <f t="shared" si="1"/>
-        <v>142.36502786121108</v>
-      </c>
-      <c r="P13" s="44">
-        <v>5.6696</v>
-      </c>
-      <c r="Q13" s="33">
+        <v>175.79282407407408</v>
+      </c>
+      <c r="P13" s="43">
+        <v>12.202199999999999</v>
+      </c>
+      <c r="Q13" s="32">
         <f t="shared" si="3"/>
-        <v>562.632623701326</v>
-      </c>
-      <c r="R13" s="33"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="20"/>
-      <c r="V13" s="20"/>
-      <c r="W13" s="20"/>
-      <c r="X13" s="20"/>
-      <c r="Y13" s="20"/>
-      <c r="Z13" s="20"/>
-      <c r="AA13" s="20"/>
-      <c r="AB13" s="20"/>
-      <c r="AC13" s="20"/>
-      <c r="AD13" s="20"/>
-      <c r="AE13" s="20"/>
-      <c r="AF13" s="20"/>
-      <c r="AG13" s="20"/>
-      <c r="AH13" s="20"/>
-      <c r="AI13" s="20"/>
-      <c r="AJ13" s="20"/>
-      <c r="AK13" s="20"/>
+        <v>706.14583333333326</v>
+      </c>
+      <c r="R13" s="32"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="38"/>
+      <c r="V13" s="38"/>
+      <c r="W13" s="38"/>
+      <c r="X13" s="38"/>
+      <c r="Y13" s="38"/>
+      <c r="Z13" s="38"/>
+      <c r="AA13" s="38"/>
+      <c r="AB13" s="38"/>
+      <c r="AC13" s="38"/>
+      <c r="AD13" s="11"/>
+      <c r="AE13" s="11"/>
+      <c r="AF13" s="11"/>
+      <c r="AG13" s="11"/>
+      <c r="AH13" s="11"/>
+      <c r="AI13" s="11"/>
+      <c r="AJ13" s="11"/>
+      <c r="AK13" s="11"/>
     </row>
     <row r="14" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="50">
@@ -2503,7 +2476,7 @@
         <v>14</v>
       </c>
       <c r="D14" s="93" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14" s="21" t="s">
         <v>47</v>
@@ -2512,34 +2485,34 @@
         <v>75</v>
       </c>
       <c r="I14" s="38">
-        <v>2.2800000000000001E-2</v>
+        <v>2.3699999999999999E-2</v>
       </c>
       <c r="J14" s="23">
-        <v>1.3120000000000001E-2</v>
+        <v>1.384E-2</v>
       </c>
       <c r="K14" s="10">
-        <v>2.2345000000000002</v>
+        <v>2.1572</v>
       </c>
       <c r="L14" s="9">
-        <v>1.9807999999999999</v>
+        <v>2.0236999999999998</v>
       </c>
       <c r="M14" s="40">
-        <v>88.644999999999996</v>
+        <v>93.798000000000002</v>
       </c>
       <c r="N14" s="40">
         <f t="shared" si="0"/>
-        <v>170.3125</v>
+        <v>155.8670520231214</v>
       </c>
       <c r="O14" s="40">
         <f t="shared" si="1"/>
-        <v>150.97560975609753</v>
+        <v>146.22109826589593</v>
       </c>
       <c r="P14" s="43">
-        <v>7.8239999999999998</v>
+        <v>7.97</v>
       </c>
       <c r="Q14" s="32">
         <f t="shared" si="3"/>
-        <v>596.34146341463406</v>
+        <v>575.86705202312135</v>
       </c>
       <c r="R14" s="32"/>
       <c r="S14" s="9"/>
@@ -2582,34 +2555,34 @@
         <v>76</v>
       </c>
       <c r="I15" s="38">
-        <v>2.8000000000000001E-2</v>
+        <v>2.1600000000000001E-2</v>
       </c>
       <c r="J15" s="23">
-        <v>1.728E-2</v>
+        <v>1.2160000000000002E-2</v>
       </c>
       <c r="K15" s="10">
-        <v>3.4662000000000002</v>
+        <v>1.8476999999999999</v>
       </c>
       <c r="L15" s="9">
-        <v>3.0377000000000001</v>
+        <v>1.7290000000000001</v>
       </c>
       <c r="M15" s="40">
-        <v>87.638000000000005</v>
+        <v>93.578000000000003</v>
       </c>
       <c r="N15" s="40">
         <f t="shared" si="0"/>
-        <v>200.59027777777777</v>
+        <v>151.94901315789471</v>
       </c>
       <c r="O15" s="40">
         <f t="shared" si="1"/>
-        <v>175.79282407407408</v>
+        <v>142.18749999999997</v>
       </c>
       <c r="P15" s="43">
-        <v>12.202199999999999</v>
+        <v>6.7137000000000002</v>
       </c>
       <c r="Q15" s="32">
         <f t="shared" si="3"/>
-        <v>706.14583333333326</v>
+        <v>552.1134868421052</v>
       </c>
       <c r="R15" s="32"/>
       <c r="S15" s="9"/>
@@ -2652,34 +2625,34 @@
         <v>77</v>
       </c>
       <c r="I16" s="38">
-        <v>2.3699999999999999E-2</v>
+        <v>1.72E-2</v>
       </c>
       <c r="J16" s="23">
-        <v>1.384E-2</v>
+        <v>8.6400000000000001E-3</v>
       </c>
       <c r="K16" s="10">
-        <v>2.1572</v>
+        <v>1.3220000000000001</v>
       </c>
       <c r="L16" s="9">
-        <v>2.0236999999999998</v>
+        <v>1.2312000000000001</v>
       </c>
       <c r="M16" s="40">
-        <v>93.798000000000002</v>
+        <v>93.135999999999996</v>
       </c>
       <c r="N16" s="40">
         <f t="shared" si="0"/>
-        <v>155.8670520231214</v>
+        <v>153.00925925925927</v>
       </c>
       <c r="O16" s="40">
         <f t="shared" si="1"/>
-        <v>146.22109826589593</v>
+        <v>142.5</v>
       </c>
       <c r="P16" s="43">
-        <v>7.97</v>
+        <v>4.8644999999999996</v>
       </c>
       <c r="Q16" s="32">
         <f t="shared" si="3"/>
-        <v>575.86705202312135</v>
+        <v>563.02083333333326</v>
       </c>
       <c r="R16" s="32"/>
       <c r="S16" s="9"/>
@@ -2702,125 +2675,93 @@
       <c r="AJ16" s="11"/>
       <c r="AK16" s="11"/>
     </row>
-    <row r="17" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="50">
+    <row r="17" spans="1:37" s="65" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="71">
         <v>44552</v>
       </c>
-      <c r="B17" s="60" t="s">
+      <c r="B17" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="93" t="s">
-        <v>74</v>
+      <c r="D17" s="94" t="s">
+        <v>73</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="56" t="s">
+      <c r="F17" s="28"/>
+      <c r="G17" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="I17" s="38">
-        <v>2.1600000000000001E-2</v>
-      </c>
-      <c r="J17" s="23">
-        <v>1.2160000000000002E-2</v>
-      </c>
-      <c r="K17" s="10">
-        <v>1.8476999999999999</v>
-      </c>
-      <c r="L17" s="9">
-        <v>1.7290000000000001</v>
-      </c>
-      <c r="M17" s="40">
-        <v>93.578000000000003</v>
-      </c>
-      <c r="N17" s="40">
+      <c r="H17" s="36"/>
+      <c r="I17" s="20">
+        <v>2.3800000000000002E-2</v>
+      </c>
+      <c r="J17" s="24">
+        <v>1.3920000000000002E-2</v>
+      </c>
+      <c r="K17" s="19">
+        <v>2.1122999999999998</v>
+      </c>
+      <c r="L17" s="18">
+        <v>2.0009000000000001</v>
+      </c>
+      <c r="M17" s="41">
+        <v>94.725999999999999</v>
+      </c>
+      <c r="N17" s="41">
         <f t="shared" si="0"/>
-        <v>151.94901315789471</v>
-      </c>
-      <c r="O17" s="40">
+        <v>151.74568965517238</v>
+      </c>
+      <c r="O17" s="41">
         <f t="shared" si="1"/>
-        <v>142.18749999999997</v>
-      </c>
-      <c r="P17" s="43">
-        <v>6.7137000000000002</v>
-      </c>
-      <c r="Q17" s="32">
+        <v>143.74281609195401</v>
+      </c>
+      <c r="P17" s="44">
+        <v>7.9024999999999999</v>
+      </c>
+      <c r="Q17" s="33">
         <f t="shared" si="3"/>
-        <v>552.1134868421052</v>
-      </c>
-      <c r="R17" s="32"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="38"/>
-      <c r="V17" s="38"/>
-      <c r="W17" s="38"/>
-      <c r="X17" s="38"/>
-      <c r="Y17" s="38"/>
-      <c r="Z17" s="38"/>
-      <c r="AA17" s="38"/>
-      <c r="AB17" s="38"/>
-      <c r="AC17" s="38"/>
-      <c r="AD17" s="11"/>
-      <c r="AE17" s="11"/>
-      <c r="AF17" s="11"/>
-      <c r="AG17" s="11"/>
-      <c r="AH17" s="11"/>
-      <c r="AI17" s="11"/>
-      <c r="AJ17" s="11"/>
-      <c r="AK17" s="11"/>
+        <v>567.70833333333326</v>
+      </c>
+      <c r="R17" s="33"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="18"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="20"/>
+      <c r="W17" s="20"/>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="20"/>
+      <c r="Z17" s="20"/>
+      <c r="AA17" s="20"/>
+      <c r="AB17" s="20"/>
+      <c r="AC17" s="20"/>
+      <c r="AD17" s="20"/>
+      <c r="AE17" s="20"/>
+      <c r="AF17" s="20"/>
+      <c r="AG17" s="20"/>
+      <c r="AH17" s="20"/>
+      <c r="AI17" s="20"/>
+      <c r="AJ17" s="20"/>
+      <c r="AK17" s="20"/>
     </row>
     <row r="18" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="50">
-        <v>44552</v>
-      </c>
-      <c r="B18" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="61" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="93" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="I18" s="38">
-        <v>1.72E-2</v>
-      </c>
-      <c r="J18" s="23">
-        <v>8.6400000000000001E-3</v>
-      </c>
-      <c r="K18" s="10">
-        <v>1.3220000000000001</v>
-      </c>
-      <c r="L18" s="9">
-        <v>1.2312000000000001</v>
-      </c>
-      <c r="M18" s="40">
-        <v>93.135999999999996</v>
-      </c>
-      <c r="N18" s="40">
-        <f t="shared" si="0"/>
-        <v>153.00925925925927</v>
-      </c>
-      <c r="O18" s="40">
-        <f t="shared" si="1"/>
-        <v>142.5</v>
-      </c>
-      <c r="P18" s="43">
-        <v>4.8644999999999996</v>
-      </c>
-      <c r="Q18" s="32">
-        <f t="shared" si="3"/>
-        <v>563.02083333333326</v>
-      </c>
+      <c r="A18" s="11"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="25"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="32"/>
       <c r="R18" s="32"/>
       <c r="S18" s="9"/>
       <c r="T18" s="9"/>
@@ -2842,77 +2783,41 @@
       <c r="AJ18" s="11"/>
       <c r="AK18" s="11"/>
     </row>
-    <row r="19" spans="1:37" s="65" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="71">
-        <v>44552</v>
-      </c>
-      <c r="B19" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="94" t="s">
-        <v>74</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="74" t="s">
-        <v>80</v>
-      </c>
-      <c r="H19" s="36"/>
-      <c r="I19" s="20">
-        <v>2.3800000000000002E-2</v>
-      </c>
-      <c r="J19" s="24">
-        <v>1.3920000000000002E-2</v>
-      </c>
-      <c r="K19" s="19">
-        <v>2.1122999999999998</v>
-      </c>
-      <c r="L19" s="18">
-        <v>2.0009000000000001</v>
-      </c>
-      <c r="M19" s="41">
-        <v>94.725999999999999</v>
-      </c>
-      <c r="N19" s="41">
-        <f t="shared" si="0"/>
-        <v>151.74568965517238</v>
-      </c>
-      <c r="O19" s="41">
-        <f t="shared" si="1"/>
-        <v>143.74281609195401</v>
-      </c>
-      <c r="P19" s="44">
-        <v>7.9024999999999999</v>
-      </c>
-      <c r="Q19" s="33">
-        <f t="shared" si="3"/>
-        <v>567.70833333333326</v>
-      </c>
-      <c r="R19" s="33"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="20"/>
-      <c r="V19" s="20"/>
-      <c r="W19" s="20"/>
-      <c r="X19" s="20"/>
-      <c r="Y19" s="20"/>
-      <c r="Z19" s="20"/>
-      <c r="AA19" s="20"/>
-      <c r="AB19" s="20"/>
-      <c r="AC19" s="20"/>
-      <c r="AD19" s="20"/>
-      <c r="AE19" s="20"/>
-      <c r="AF19" s="20"/>
-      <c r="AG19" s="20"/>
-      <c r="AH19" s="20"/>
-      <c r="AI19" s="20"/>
-      <c r="AJ19" s="20"/>
-      <c r="AK19" s="20"/>
+    <row r="19" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="11"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="25"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="38"/>
+      <c r="V19" s="38"/>
+      <c r="W19" s="38"/>
+      <c r="X19" s="38"/>
+      <c r="Y19" s="38"/>
+      <c r="Z19" s="38"/>
+      <c r="AA19" s="38"/>
+      <c r="AB19" s="38"/>
+      <c r="AC19" s="38"/>
+      <c r="AD19" s="11"/>
+      <c r="AE19" s="11"/>
+      <c r="AF19" s="11"/>
+      <c r="AG19" s="11"/>
+      <c r="AH19" s="11"/>
+      <c r="AI19" s="11"/>
+      <c r="AJ19" s="11"/>
+      <c r="AK19" s="11"/>
     </row>
     <row r="20" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="11"/>
@@ -26170,77 +26075,19 @@
       <c r="AJ665" s="11"/>
       <c r="AK665" s="11"/>
     </row>
-    <row r="666" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="666" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A666" s="11"/>
       <c r="B666" s="46"/>
       <c r="C666" s="8"/>
       <c r="D666" s="13"/>
       <c r="E666" s="25"/>
-      <c r="I666" s="38"/>
-      <c r="J666" s="23"/>
-      <c r="K666" s="10"/>
-      <c r="L666" s="9"/>
-      <c r="M666" s="40"/>
-      <c r="N666" s="40"/>
-      <c r="O666" s="40"/>
-      <c r="P666" s="43"/>
-      <c r="Q666" s="32"/>
-      <c r="R666" s="32"/>
-      <c r="S666" s="9"/>
-      <c r="T666" s="9"/>
-      <c r="U666" s="38"/>
-      <c r="V666" s="38"/>
-      <c r="W666" s="38"/>
-      <c r="X666" s="38"/>
-      <c r="Y666" s="38"/>
-      <c r="Z666" s="38"/>
-      <c r="AA666" s="38"/>
-      <c r="AB666" s="38"/>
-      <c r="AC666" s="38"/>
-      <c r="AD666" s="11"/>
-      <c r="AE666" s="11"/>
-      <c r="AF666" s="11"/>
-      <c r="AG666" s="11"/>
-      <c r="AH666" s="11"/>
-      <c r="AI666" s="11"/>
-      <c r="AJ666" s="11"/>
-      <c r="AK666" s="11"/>
-    </row>
-    <row r="667" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="667" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A667" s="11"/>
       <c r="B667" s="46"/>
       <c r="C667" s="8"/>
       <c r="D667" s="13"/>
       <c r="E667" s="25"/>
-      <c r="I667" s="38"/>
-      <c r="J667" s="23"/>
-      <c r="K667" s="10"/>
-      <c r="L667" s="9"/>
-      <c r="M667" s="40"/>
-      <c r="N667" s="40"/>
-      <c r="O667" s="40"/>
-      <c r="P667" s="43"/>
-      <c r="Q667" s="32"/>
-      <c r="R667" s="32"/>
-      <c r="S667" s="9"/>
-      <c r="T667" s="9"/>
-      <c r="U667" s="38"/>
-      <c r="V667" s="38"/>
-      <c r="W667" s="38"/>
-      <c r="X667" s="38"/>
-      <c r="Y667" s="38"/>
-      <c r="Z667" s="38"/>
-      <c r="AA667" s="38"/>
-      <c r="AB667" s="38"/>
-      <c r="AC667" s="38"/>
-      <c r="AD667" s="11"/>
-      <c r="AE667" s="11"/>
-      <c r="AF667" s="11"/>
-      <c r="AG667" s="11"/>
-      <c r="AH667" s="11"/>
-      <c r="AI667" s="11"/>
-      <c r="AJ667" s="11"/>
-      <c r="AK667" s="11"/>
     </row>
     <row r="668" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A668" s="11"/>
@@ -26270,114 +26117,90 @@
       <c r="D671" s="13"/>
       <c r="E671" s="25"/>
     </row>
-    <row r="672" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A672" s="11"/>
-      <c r="B672" s="46"/>
-      <c r="C672" s="8"/>
-      <c r="D672" s="13"/>
-      <c r="E672" s="25"/>
-    </row>
-    <row r="673" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A673" s="11"/>
-      <c r="B673" s="46"/>
-      <c r="C673" s="8"/>
-      <c r="D673" s="13"/>
-      <c r="E673" s="25"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B20:B1048576">
-    <cfRule type="containsText" dxfId="38" priority="256" operator="containsText" text="Lithium">
+  <conditionalFormatting sqref="B1 B18:B1048576">
+    <cfRule type="containsText" dxfId="36" priority="256" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH("Lithium",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="37" priority="18" operator="containsText" text="Lithium">
+    <cfRule type="containsText" dxfId="35" priority="18" operator="containsText" text="Lithium">
+      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B97))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="containsText" dxfId="34" priority="16" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B99))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="containsText" dxfId="36" priority="17" operator="containsText" text="Lithium">
+  <conditionalFormatting sqref="B4">
+    <cfRule type="containsText" dxfId="33" priority="15" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B100))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4">
-    <cfRule type="containsText" dxfId="35" priority="16" operator="containsText" text="Lithium">
+  <conditionalFormatting sqref="B5">
+    <cfRule type="containsText" dxfId="32" priority="14" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B101))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5">
-    <cfRule type="containsText" dxfId="34" priority="15" operator="containsText" text="Lithium">
+  <conditionalFormatting sqref="B6">
+    <cfRule type="containsText" dxfId="31" priority="13" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B102))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="containsText" dxfId="33" priority="14" operator="containsText" text="Lithium">
+  <conditionalFormatting sqref="B7">
+    <cfRule type="containsText" dxfId="30" priority="12" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B103))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="containsText" dxfId="32" priority="13" operator="containsText" text="Lithium">
+  <conditionalFormatting sqref="B8">
+    <cfRule type="containsText" dxfId="29" priority="11" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B104))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8">
-    <cfRule type="containsText" dxfId="31" priority="12" operator="containsText" text="Lithium">
+  <conditionalFormatting sqref="B9">
+    <cfRule type="containsText" dxfId="28" priority="10" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B105))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="containsText" dxfId="30" priority="11" operator="containsText" text="Lithium">
+  <conditionalFormatting sqref="B10">
+    <cfRule type="containsText" dxfId="27" priority="9" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B106))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10">
-    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Lithium">
+  <conditionalFormatting sqref="B11">
+    <cfRule type="containsText" dxfId="26" priority="8" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B107))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11">
-    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Lithium">
+  <conditionalFormatting sqref="B12">
+    <cfRule type="containsText" dxfId="25" priority="7" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B108))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
-    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="Lithium">
-      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B109))))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="Lithium">
+    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B110))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="Lithium">
+    <cfRule type="containsText" dxfId="22" priority="4" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B111))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="24" priority="5" operator="containsText" text="Lithium">
+    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B112))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Lithium">
+    <cfRule type="containsText" dxfId="20" priority="2" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B113))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="Lithium">
+    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B114))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="Lithium">
-      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B115))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Lithium">
-      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B116))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -26387,11 +26210,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AG669"/>
+  <dimension ref="A1:AG668"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -26632,7 +26455,7 @@
         <v>4</v>
       </c>
       <c r="I3" s="56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J3" s="58">
         <v>6.4000000000000003E-3</v>
@@ -26721,7 +26544,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="56" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J4" s="58">
         <v>6.4000000000000003E-3</v>
@@ -26730,14 +26553,14 @@
         <v>2.12E-2</v>
       </c>
       <c r="L4" s="53">
-        <f t="shared" ref="L4:L18" si="11">K4-J4</f>
+        <f t="shared" ref="L4:L17" si="11">K4-J4</f>
         <v>1.4800000000000001E-2</v>
       </c>
       <c r="M4" s="53">
         <v>0.76922999999999997</v>
       </c>
       <c r="N4" s="54">
-        <f t="shared" ref="N4:N18" si="12">L4*M4</f>
+        <f t="shared" ref="N4:N17" si="12">L4*M4</f>
         <v>1.1384604E-2</v>
       </c>
       <c r="O4" s="53">
@@ -26747,42 +26570,42 @@
         <v>1.538</v>
       </c>
       <c r="Q4" s="62">
-        <f t="shared" ref="Q4:Q18" si="13">N4*O4/1000</f>
+        <f t="shared" ref="Q4:Q17" si="13">N4*O4/1000</f>
         <v>1.7076905999999998E-3</v>
       </c>
       <c r="R4" s="63">
-        <f t="shared" ref="R4:R18" si="14">Q4/10</f>
+        <f t="shared" ref="R4:R17" si="14">Q4/10</f>
         <v>1.7076905999999998E-4</v>
       </c>
       <c r="S4" s="53">
-        <f t="shared" ref="S4:S18" si="15">Q4/3</f>
+        <f t="shared" ref="S4:S17" si="15">Q4/3</f>
         <v>5.6923019999999996E-4</v>
       </c>
       <c r="T4" s="62">
-        <f t="shared" ref="T4:T18" si="16">Q4/2</f>
+        <f t="shared" ref="T4:T17" si="16">Q4/2</f>
         <v>8.5384529999999988E-4</v>
       </c>
       <c r="U4" s="64">
-        <f t="shared" ref="U4:U18" si="17">R4/2</f>
+        <f t="shared" ref="U4:U17" si="17">R4/2</f>
         <v>8.5384529999999991E-5</v>
       </c>
       <c r="V4" s="64">
-        <f t="shared" ref="V4:V18" si="18">R4/5</f>
+        <f t="shared" ref="V4:V17" si="18">R4/5</f>
         <v>3.4153811999999998E-5</v>
       </c>
       <c r="W4" s="53">
-        <f t="shared" ref="W4:W18" si="19">0.7*Q4</f>
+        <f t="shared" ref="W4:W17" si="19">0.7*Q4</f>
         <v>1.1953834199999998E-3</v>
       </c>
       <c r="X4" s="96">
-        <f t="shared" ref="X4:X18" si="20">V4*10</f>
+        <f t="shared" ref="X4:X17" si="20">V4*10</f>
         <v>3.4153811999999996E-4</v>
       </c>
       <c r="Y4" s="56">
         <v>1.4285000000000001</v>
       </c>
       <c r="Z4" s="57">
-        <f t="shared" ref="Z4:Z18" si="21">N4*O4/P4</f>
+        <f t="shared" ref="Z4:Z17" si="21">N4*O4/P4</f>
         <v>1.1103319895968788</v>
       </c>
     </row>
@@ -26810,7 +26633,7 @@
         <v>6</v>
       </c>
       <c r="I5" s="56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J5" s="58">
         <v>6.4000000000000003E-3</v>
@@ -26899,7 +26722,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="56" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J6" s="58">
         <v>6.4000000000000003E-3</v>
@@ -26988,7 +26811,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J7" s="58">
         <v>6.4000000000000003E-3</v>
@@ -27077,7 +26900,7 @@
         <v>3</v>
       </c>
       <c r="I8" s="56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J8" s="58">
         <v>6.4000000000000003E-3</v>
@@ -27166,7 +26989,7 @@
         <v>5</v>
       </c>
       <c r="I9" s="56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J9" s="58">
         <v>6.4000000000000003E-3</v>
@@ -27255,7 +27078,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J10" s="58">
         <v>6.4000000000000003E-3</v>
@@ -27344,7 +27167,7 @@
         <v>4</v>
       </c>
       <c r="I11" s="56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J11" s="58">
         <v>6.4000000000000003E-3</v>
@@ -27432,7 +27255,7 @@
         <v>6</v>
       </c>
       <c r="I12" s="74" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J12" s="76">
         <v>6.4000000000000003E-3</v>
@@ -27508,37 +27331,37 @@
         <v>14</v>
       </c>
       <c r="D13" s="93" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" s="51" t="s">
         <v>47</v>
       </c>
       <c r="F13" s="87"/>
       <c r="G13" s="89">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13" s="52">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I13" s="56" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J13" s="58">
         <v>6.4000000000000003E-3</v>
       </c>
       <c r="K13" s="59">
-        <v>2.2800000000000001E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="L13" s="53">
         <f t="shared" si="11"/>
-        <v>1.6400000000000001E-2</v>
+        <v>2.1600000000000001E-2</v>
       </c>
       <c r="M13" s="53">
         <v>0.8</v>
       </c>
       <c r="N13" s="54">
         <f t="shared" si="12"/>
-        <v>1.3120000000000001E-2</v>
+        <v>1.728E-2</v>
       </c>
       <c r="O13" s="53">
         <v>150</v>
@@ -27548,42 +27371,42 @@
       </c>
       <c r="Q13" s="62">
         <f t="shared" si="13"/>
-        <v>1.9680000000000001E-3</v>
+        <v>2.5920000000000001E-3</v>
       </c>
       <c r="R13" s="63">
         <f t="shared" si="14"/>
-        <v>1.9680000000000001E-4</v>
+        <v>2.5920000000000001E-4</v>
       </c>
       <c r="S13" s="53">
         <f t="shared" si="15"/>
-        <v>6.5600000000000001E-4</v>
+        <v>8.6400000000000008E-4</v>
       </c>
       <c r="T13" s="62">
         <f t="shared" si="16"/>
-        <v>9.8400000000000007E-4</v>
+        <v>1.2960000000000001E-3</v>
       </c>
       <c r="U13" s="64">
         <f t="shared" si="17"/>
-        <v>9.8400000000000007E-5</v>
+        <v>1.2960000000000001E-4</v>
       </c>
       <c r="V13" s="64">
         <f t="shared" si="18"/>
-        <v>3.9360000000000003E-5</v>
+        <v>5.1840000000000005E-5</v>
       </c>
       <c r="W13" s="53">
         <f t="shared" si="19"/>
-        <v>1.3776000000000001E-3</v>
+        <v>1.8143999999999999E-3</v>
       </c>
       <c r="X13" s="96">
         <f t="shared" si="20"/>
-        <v>3.9360000000000003E-4</v>
+        <v>5.1840000000000002E-4</v>
       </c>
       <c r="Y13" s="56">
-        <v>1.6721999999999999</v>
+        <v>1.395</v>
       </c>
       <c r="Z13" s="57">
         <f t="shared" si="21"/>
-        <v>1.2795838751625488</v>
+        <v>1.6853055916775033</v>
       </c>
     </row>
     <row r="14" spans="1:33" s="56" customFormat="1" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -27597,37 +27420,37 @@
         <v>14</v>
       </c>
       <c r="D14" s="93" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14" s="51" t="s">
         <v>47</v>
       </c>
       <c r="F14" s="87"/>
       <c r="G14" s="89">
+        <v>3</v>
+      </c>
+      <c r="H14" s="52">
         <v>2</v>
       </c>
-      <c r="H14" s="52">
-        <v>4</v>
-      </c>
       <c r="I14" s="56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J14" s="58">
         <v>6.4000000000000003E-3</v>
       </c>
       <c r="K14" s="59">
-        <v>2.8000000000000001E-2</v>
+        <v>2.3699999999999999E-2</v>
       </c>
       <c r="L14" s="53">
         <f t="shared" si="11"/>
-        <v>2.1600000000000001E-2</v>
+        <v>1.7299999999999999E-2</v>
       </c>
       <c r="M14" s="53">
         <v>0.8</v>
       </c>
       <c r="N14" s="54">
         <f t="shared" si="12"/>
-        <v>1.728E-2</v>
+        <v>1.384E-2</v>
       </c>
       <c r="O14" s="53">
         <v>150</v>
@@ -27637,42 +27460,42 @@
       </c>
       <c r="Q14" s="62">
         <f t="shared" si="13"/>
-        <v>2.5920000000000001E-3</v>
+        <v>2.0760000000000002E-3</v>
       </c>
       <c r="R14" s="63">
         <f t="shared" si="14"/>
-        <v>2.5920000000000001E-4</v>
+        <v>2.076E-4</v>
       </c>
       <c r="S14" s="53">
         <f t="shared" si="15"/>
-        <v>8.6400000000000008E-4</v>
+        <v>6.9200000000000002E-4</v>
       </c>
       <c r="T14" s="62">
         <f t="shared" si="16"/>
-        <v>1.2960000000000001E-3</v>
+        <v>1.0380000000000001E-3</v>
       </c>
       <c r="U14" s="64">
         <f t="shared" si="17"/>
-        <v>1.2960000000000001E-4</v>
+        <v>1.038E-4</v>
       </c>
       <c r="V14" s="64">
         <f t="shared" si="18"/>
-        <v>5.1840000000000005E-5</v>
+        <v>4.1520000000000002E-5</v>
       </c>
       <c r="W14" s="53">
         <f t="shared" si="19"/>
-        <v>1.8143999999999999E-3</v>
+        <v>1.4532E-3</v>
       </c>
       <c r="X14" s="96">
         <f t="shared" si="20"/>
-        <v>5.1840000000000002E-4</v>
+        <v>4.1520000000000001E-4</v>
       </c>
       <c r="Y14" s="56">
-        <v>1.395</v>
+        <v>1.5007999999999999</v>
       </c>
       <c r="Z14" s="57">
         <f t="shared" si="21"/>
-        <v>1.6853055916775033</v>
+        <v>1.3498049414824447</v>
       </c>
     </row>
     <row r="15" spans="1:33" s="56" customFormat="1" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -27696,27 +27519,27 @@
         <v>3</v>
       </c>
       <c r="H15" s="52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I15" s="56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J15" s="58">
         <v>6.4000000000000003E-3</v>
       </c>
       <c r="K15" s="59">
-        <v>2.3699999999999999E-2</v>
+        <v>2.1600000000000001E-2</v>
       </c>
       <c r="L15" s="53">
         <f t="shared" si="11"/>
-        <v>1.7299999999999999E-2</v>
+        <v>1.5200000000000002E-2</v>
       </c>
       <c r="M15" s="53">
         <v>0.8</v>
       </c>
       <c r="N15" s="54">
         <f t="shared" si="12"/>
-        <v>1.384E-2</v>
+        <v>1.2160000000000002E-2</v>
       </c>
       <c r="O15" s="53">
         <v>150</v>
@@ -27726,42 +27549,42 @@
       </c>
       <c r="Q15" s="62">
         <f t="shared" si="13"/>
-        <v>2.0760000000000002E-3</v>
+        <v>1.8240000000000003E-3</v>
       </c>
       <c r="R15" s="63">
         <f t="shared" si="14"/>
-        <v>2.076E-4</v>
+        <v>1.8240000000000004E-4</v>
       </c>
       <c r="S15" s="53">
         <f t="shared" si="15"/>
-        <v>6.9200000000000002E-4</v>
+        <v>6.0800000000000014E-4</v>
       </c>
       <c r="T15" s="62">
         <f t="shared" si="16"/>
-        <v>1.0380000000000001E-3</v>
+        <v>9.1200000000000016E-4</v>
       </c>
       <c r="U15" s="64">
         <f t="shared" si="17"/>
-        <v>1.038E-4</v>
+        <v>9.1200000000000021E-5</v>
       </c>
       <c r="V15" s="64">
         <f t="shared" si="18"/>
-        <v>4.1520000000000002E-5</v>
+        <v>3.648000000000001E-5</v>
       </c>
       <c r="W15" s="53">
         <f t="shared" si="19"/>
-        <v>1.4532E-3</v>
+        <v>1.2768000000000002E-3</v>
       </c>
       <c r="X15" s="96">
         <f t="shared" si="20"/>
-        <v>4.1520000000000001E-4</v>
+        <v>3.6480000000000009E-4</v>
       </c>
       <c r="Y15" s="56">
-        <v>1.5007999999999999</v>
+        <v>1.6377999999999999</v>
       </c>
       <c r="Z15" s="57">
         <f t="shared" si="21"/>
-        <v>1.3498049414824447</v>
+        <v>1.1859557867360209</v>
       </c>
     </row>
     <row r="16" spans="1:33" s="56" customFormat="1" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -27775,37 +27598,37 @@
         <v>14</v>
       </c>
       <c r="D16" s="93" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16" s="51" t="s">
         <v>47</v>
       </c>
       <c r="F16" s="87"/>
       <c r="G16" s="89">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H16" s="52">
         <v>3</v>
       </c>
       <c r="I16" s="56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J16" s="58">
         <v>6.4000000000000003E-3</v>
       </c>
       <c r="K16" s="59">
-        <v>2.1600000000000001E-2</v>
+        <v>1.72E-2</v>
       </c>
       <c r="L16" s="53">
         <f t="shared" si="11"/>
-        <v>1.5200000000000002E-2</v>
+        <v>1.0800000000000001E-2</v>
       </c>
       <c r="M16" s="53">
         <v>0.8</v>
       </c>
       <c r="N16" s="54">
         <f t="shared" si="12"/>
-        <v>1.2160000000000002E-2</v>
+        <v>8.6400000000000001E-3</v>
       </c>
       <c r="O16" s="53">
         <v>150</v>
@@ -27815,220 +27638,160 @@
       </c>
       <c r="Q16" s="62">
         <f t="shared" si="13"/>
-        <v>1.8240000000000003E-3</v>
+        <v>1.2960000000000001E-3</v>
       </c>
       <c r="R16" s="63">
         <f t="shared" si="14"/>
-        <v>1.8240000000000004E-4</v>
+        <v>1.2960000000000001E-4</v>
       </c>
       <c r="S16" s="53">
         <f t="shared" si="15"/>
-        <v>6.0800000000000014E-4</v>
+        <v>4.3200000000000004E-4</v>
       </c>
       <c r="T16" s="62">
         <f t="shared" si="16"/>
-        <v>9.1200000000000016E-4</v>
+        <v>6.4800000000000003E-4</v>
       </c>
       <c r="U16" s="64">
         <f t="shared" si="17"/>
-        <v>9.1200000000000021E-5</v>
+        <v>6.4800000000000003E-5</v>
       </c>
       <c r="V16" s="64">
         <f t="shared" si="18"/>
-        <v>3.648000000000001E-5</v>
+        <v>2.5920000000000003E-5</v>
       </c>
       <c r="W16" s="53">
         <f t="shared" si="19"/>
-        <v>1.2768000000000002E-3</v>
+        <v>9.0719999999999993E-4</v>
       </c>
       <c r="X16" s="96">
         <f t="shared" si="20"/>
-        <v>3.6480000000000009E-4</v>
+        <v>2.5920000000000001E-4</v>
       </c>
       <c r="Y16" s="56">
-        <v>1.6377999999999999</v>
+        <v>2.0808499999999999</v>
       </c>
       <c r="Z16" s="57">
         <f t="shared" si="21"/>
-        <v>1.1859557867360209</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" s="56" customFormat="1" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+        <v>0.84265279583875163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" s="74" customFormat="1" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="50">
         <v>44552</v>
       </c>
-      <c r="B17" s="60" t="s">
+      <c r="B17" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="93" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="51" t="s">
+      <c r="D17" s="94" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="87"/>
-      <c r="G17" s="89">
-        <v>4</v>
-      </c>
-      <c r="H17" s="52">
-        <v>3</v>
-      </c>
-      <c r="I17" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="J17" s="58">
+      <c r="G17" s="90">
+        <v>6</v>
+      </c>
+      <c r="H17" s="75">
+        <v>1</v>
+      </c>
+      <c r="I17" s="74" t="s">
+        <v>78</v>
+      </c>
+      <c r="J17" s="76">
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="K17" s="59">
-        <v>1.72E-2</v>
-      </c>
-      <c r="L17" s="53">
-        <f t="shared" si="11"/>
-        <v>1.0800000000000001E-2</v>
-      </c>
-      <c r="M17" s="53">
-        <v>0.8</v>
-      </c>
-      <c r="N17" s="54">
-        <f t="shared" si="12"/>
-        <v>8.6400000000000001E-3</v>
-      </c>
-      <c r="O17" s="53">
-        <v>150</v>
-      </c>
-      <c r="P17" s="55">
-        <v>1.538</v>
-      </c>
-      <c r="Q17" s="62">
-        <f t="shared" si="13"/>
-        <v>1.2960000000000001E-3</v>
-      </c>
-      <c r="R17" s="63">
-        <f t="shared" si="14"/>
-        <v>1.2960000000000001E-4</v>
-      </c>
-      <c r="S17" s="53">
-        <f t="shared" si="15"/>
-        <v>4.3200000000000004E-4</v>
-      </c>
-      <c r="T17" s="62">
-        <f t="shared" si="16"/>
-        <v>6.4800000000000003E-4</v>
-      </c>
-      <c r="U17" s="64">
-        <f t="shared" si="17"/>
-        <v>6.4800000000000003E-5</v>
-      </c>
-      <c r="V17" s="64">
-        <f t="shared" si="18"/>
-        <v>2.5920000000000003E-5</v>
-      </c>
-      <c r="W17" s="53">
-        <f t="shared" si="19"/>
-        <v>9.0719999999999993E-4</v>
-      </c>
-      <c r="X17" s="96">
-        <f t="shared" si="20"/>
-        <v>2.5920000000000001E-4</v>
-      </c>
-      <c r="Y17" s="56">
-        <v>2.0808499999999999</v>
-      </c>
-      <c r="Z17" s="57">
-        <f t="shared" si="21"/>
-        <v>0.84265279583875163</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" s="74" customFormat="1" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="50">
-        <v>44552</v>
-      </c>
-      <c r="B18" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="94" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" s="90">
-        <v>6</v>
-      </c>
-      <c r="H18" s="75">
-        <v>1</v>
-      </c>
-      <c r="I18" s="74" t="s">
-        <v>80</v>
-      </c>
-      <c r="J18" s="76">
-        <v>6.4000000000000003E-3</v>
-      </c>
-      <c r="K18" s="77">
+      <c r="K17" s="77">
         <v>2.3800000000000002E-2</v>
       </c>
-      <c r="L18" s="78">
+      <c r="L17" s="78">
         <f t="shared" si="11"/>
         <v>1.7400000000000002E-2</v>
       </c>
-      <c r="M18" s="78">
+      <c r="M17" s="78">
         <v>0.8</v>
       </c>
-      <c r="N18" s="79">
+      <c r="N17" s="79">
         <f t="shared" si="12"/>
         <v>1.3920000000000002E-2</v>
       </c>
-      <c r="O18" s="78">
+      <c r="O17" s="78">
         <v>150</v>
       </c>
-      <c r="P18" s="80">
+      <c r="P17" s="80">
         <v>1.538</v>
       </c>
-      <c r="Q18" s="81">
+      <c r="Q17" s="81">
         <f t="shared" si="13"/>
         <v>2.088E-3</v>
       </c>
-      <c r="R18" s="82">
+      <c r="R17" s="82">
         <f t="shared" si="14"/>
         <v>2.0880000000000001E-4</v>
       </c>
-      <c r="S18" s="78">
+      <c r="S17" s="78">
         <f t="shared" si="15"/>
         <v>6.96E-4</v>
       </c>
-      <c r="T18" s="81">
+      <c r="T17" s="81">
         <f t="shared" si="16"/>
         <v>1.044E-3</v>
       </c>
-      <c r="U18" s="83">
+      <c r="U17" s="83">
         <f t="shared" si="17"/>
         <v>1.044E-4</v>
       </c>
-      <c r="V18" s="83">
+      <c r="V17" s="83">
         <f t="shared" si="18"/>
         <v>4.176E-5</v>
       </c>
-      <c r="W18" s="78">
+      <c r="W17" s="78">
         <f t="shared" si="19"/>
         <v>1.4616E-3</v>
       </c>
-      <c r="X18" s="97">
+      <c r="X17" s="97">
         <f t="shared" si="20"/>
         <v>4.1760000000000001E-4</v>
       </c>
-      <c r="Y18" s="74">
+      <c r="Y17" s="74">
         <v>2.298</v>
       </c>
-      <c r="Z18" s="84">
+      <c r="Z17" s="84">
         <f t="shared" si="21"/>
         <v>1.3576072821846554</v>
       </c>
+    </row>
+    <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="11"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="11"/>
@@ -46851,128 +46614,94 @@
       <c r="Z667" s="11"/>
       <c r="AA667" s="11"/>
     </row>
-    <row r="668" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A668" s="11"/>
-      <c r="B668" s="12"/>
-      <c r="C668" s="92"/>
-      <c r="D668" s="95"/>
-      <c r="E668" s="15"/>
-      <c r="F668" s="38"/>
-      <c r="G668" s="32"/>
-      <c r="H668" s="11"/>
-      <c r="I668" s="29"/>
-      <c r="J668" s="11"/>
-      <c r="K668" s="16"/>
-      <c r="L668" s="11"/>
+    <row r="668" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="M668" s="11"/>
-      <c r="N668" s="11"/>
-      <c r="O668" s="11"/>
-      <c r="P668" s="11"/>
-      <c r="Q668" s="11"/>
-      <c r="R668" s="11"/>
-      <c r="S668" s="11"/>
-      <c r="T668" s="11"/>
-      <c r="U668" s="11"/>
-      <c r="V668" s="11"/>
-      <c r="W668" s="11"/>
-      <c r="X668" s="11"/>
-      <c r="Y668" s="11"/>
-      <c r="Z668" s="11"/>
-      <c r="AA668" s="11"/>
-    </row>
-    <row r="669" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="M669" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="B19:B668">
-    <cfRule type="containsText" dxfId="19" priority="272" operator="containsText" text="Lithium">
-      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B116))))</formula>
+  <conditionalFormatting sqref="B18:B667">
+    <cfRule type="containsText" dxfId="18" priority="272" operator="containsText" text="Lithium">
+      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B115))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Lithium">
-      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B98))))</formula>
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="Lithium">
+      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B97))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
     <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="Lithium">
-      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B100))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B99))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
     <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Lithium">
-      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B101))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B100))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
     <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="Lithium">
-      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B102))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B101))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
     <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Lithium">
-      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B103))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B102))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
     <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Lithium">
-      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B104))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B103))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
     <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="Lithium">
-      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B105))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B104))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
     <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="Lithium">
-      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B106))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B105))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
     <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Lithium">
-      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B107))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B106))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
     <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="Lithium">
-      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B108))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B107))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
     <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Lithium">
-      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B109))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B108))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Lithium">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B110))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Lithium">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B111))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Lithium">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B112))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Lithium">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B113))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Lithium">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Lithium">
       <formula>NOT(ISERROR(SEARCH(("Lithium"),(B114))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Lithium">
-      <formula>NOT(ISERROR(SEARCH(("Lithium"),(B115))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">

</xml_diff>